<commit_message>
updated the game logic to be scalable up to 5x5. There are a few bugs where the game throws up a winner when it's not complete, this is possibly due to the numbers getting too large and the bitwise operator is finding similar strings of e.g. 1111 within other binary values i.e. 10010110111.110010110 <<< note that around the decimal point there are 5 consecutive 1's and this sometimes incorrectly triggers the 'winner' function. I changed each cell value to be HALF of the previous cell instead of double. this seems to have solved the issue. however when the game is won with 2 tiles remaining, the board still remains active. possible solution: make the 1st cell value worth 2toPowerOf13 so that values of cells do not become too large or too small across the board.
</commit_message>
<xml_diff>
--- a/resources/calculate_winningScores.xlsx
+++ b/resources/calculate_winningScores.xlsx
@@ -16,6 +16,9 @@
     <sheet name="4x4" sheetId="4" r:id="rId2"/>
     <sheet name="5x5" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'5x5'!$P$2:$S$12</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -52,16 +55,16 @@
     <t>Concatenate:</t>
   </si>
   <si>
+    <t>,",",</t>
+  </si>
+  <si>
     <t>FINAL:</t>
   </si>
   <si>
-    <t>," , ",</t>
+    <t>Text format:</t>
   </si>
   <si>
-    <t>1057 , 2114 , 4228 , 8456 , 16912 , 33824 , 67648 , 135296 , 270592 , 541184 , 1082368 , 2164736 , 4329472 , 8658944 , 17317888 , 7 , 224 , 7168 , 229376 , 7340032 , 14 , 448 , 14336 , 458752 , 14680064 , 28 , 896 , 28672 , 917504 , 29360128 , 4161 , 8322 , 16644 , 133152 , 266304 , 532608 , 4260864 , 8521728 , 17043456 , 1092 , 2184 , 4368 , 34944 , 69888 , 139776 , 2236416 , 4472832</t>
-  </si>
-  <si>
-    <t>Text format:</t>
+    <t>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -147,19 +150,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -439,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -465,7 +455,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -474,7 +464,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -498,12 +488,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,49 +506,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -846,7 +833,7 @@
   <dimension ref="B1:J7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -856,27 +843,27 @@
   <sheetData>
     <row r="1" spans="2:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <f>B2*2</f>
         <v>2</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <f>C2*2</f>
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <f>B2+C3+D4</f>
         <v>273</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <f>D2*2</f>
         <v>8</v>
       </c>
@@ -884,43 +871,43 @@
         <f>B3*2</f>
         <v>16</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <f>C3*2</f>
         <v>32</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <f>B4+C3+D2</f>
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <f>D3*2</f>
         <v>64</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="18">
         <f>B4*2</f>
         <v>128</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="19">
         <f>C4*2</f>
         <v>256</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <f>B2+B3+B4</f>
         <v>73</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <f>C2+C3+C4</f>
         <v>146</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <f>D2+D3+D4</f>
         <v>292</v>
       </c>
@@ -929,19 +916,19 @@
       <c r="G5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <f>B2+C2+D2</f>
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <f>B3+C3+D3</f>
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <f>B4+C4+D4</f>
         <v>448</v>
       </c>
@@ -957,7 +944,7 @@
   <dimension ref="B1:O7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -967,54 +954,54 @@
   <sheetData>
     <row r="1" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <f>B2*2</f>
         <v>2</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <f>C2*2</f>
         <v>4</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <f>D2*2</f>
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="22">
         <f>B2+C3+D4</f>
         <v>1057</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <f>C2+D3+E4</f>
         <v>2114</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="22">
+      <c r="L2" s="21">
         <f>B2+B3+B4</f>
         <v>273</v>
       </c>
-      <c r="M2" s="23">
+      <c r="M2" s="22">
         <f t="shared" ref="M2:O2" si="0">C2+C3+C4</f>
         <v>546</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="22">
         <f t="shared" si="0"/>
         <v>1092</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="11">
         <f t="shared" si="0"/>
         <v>2184</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <f>E2*2</f>
         <v>16</v>
       </c>
@@ -1026,38 +1013,38 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="8">
+      <c r="G3" s="20"/>
+      <c r="H3" s="7">
         <f>B3+C4+D5</f>
         <v>16912</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="23">
         <f>C3+D4+E5</f>
         <v>33824</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="24">
         <f>B3+B4+B5</f>
         <v>4368</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="20">
         <f t="shared" ref="M3" si="2">C3+C4+C5</f>
         <v>8736</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="8">
         <f t="shared" ref="N3" si="3">D3+D4+D5</f>
         <v>17472</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="23">
         <f t="shared" ref="O3" si="4">E3+E4+E5</f>
         <v>34944</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <f t="shared" ref="B4:B5" si="5">E3*2</f>
         <v>256</v>
       </c>
@@ -1069,87 +1056,87 @@
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="22">
         <f>B4+C3+D2</f>
         <v>292</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <f>C4+D3+E2</f>
         <v>584</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="21">
         <f>B2+C2+D2</f>
         <v>7</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f>C2+D2+E2</f>
         <v>14</v>
       </c>
-      <c r="N4" s="21"/>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <f t="shared" si="5"/>
         <v>4096</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="19">
         <f t="shared" si="1"/>
         <v>32768</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f>B5+C4+D3</f>
         <v>4672</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="23">
         <f>C5+D4+E3</f>
         <v>9344</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="25">
+      <c r="K5" s="20"/>
+      <c r="L5" s="24">
         <f>B3+C3+D3</f>
         <v>112</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="25">
         <f>C3+D3+E3</f>
         <v>224</v>
       </c>
-      <c r="N5" s="21"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K6" s="21"/>
-      <c r="L6" s="25">
+      <c r="K6" s="20"/>
+      <c r="L6" s="24">
         <f>B4+C4+D4</f>
         <v>1792</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="25">
         <f>C4+D4+E4</f>
         <v>3584</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <f>B5+C5+D5</f>
         <v>28672</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="23">
         <f>C5+D5+E5</f>
         <v>57344</v>
       </c>
@@ -1163,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J8" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1188,45 +1175,45 @@
   <sheetData>
     <row r="1" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>1</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <f>C2*2</f>
         <v>2</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="31">
         <f>D2*2</f>
         <v>4</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="31">
         <f>E2*2</f>
         <v>8</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="32">
         <f>F2*2</f>
         <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="22">
+      <c r="J2" s="21">
         <f>C2+C3+C4</f>
         <v>1057</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="22">
         <f t="shared" ref="K2:N4" si="0">D2+D3+D4</f>
         <v>2114</v>
       </c>
-      <c r="L2" s="23">
+      <c r="L2" s="22">
         <f t="shared" si="0"/>
         <v>4228</v>
       </c>
-      <c r="M2" s="23">
+      <c r="M2" s="22">
         <f t="shared" si="0"/>
         <v>8456</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="11">
         <f t="shared" si="0"/>
         <v>16912</v>
       </c>
@@ -1234,12 +1221,12 @@
         <v>6</v>
       </c>
       <c r="Q2" s="2" t="str">
-        <f>CONCATENATE(J2, " , ", K2, " , ", L2, " , ", M2, " , ", N2)</f>
-        <v>1057 , 2114 , 4228 , 8456 , 16912</v>
+        <f>CONCATENATE(J2, ",", K2, ",", L2, ",", M2, ",", N2)</f>
+        <v>1057,2114,4228,8456,16912</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="34">
+      <c r="C3" s="33">
         <f>G2*2</f>
         <v>32</v>
       </c>
@@ -1255,40 +1242,40 @@
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="16">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="24">
         <f t="shared" ref="J3:J4" si="2">C3+C4+C5</f>
         <v>33824</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="20">
         <f t="shared" si="0"/>
         <v>67648</v>
       </c>
-      <c r="L3" s="21">
+      <c r="L3" s="20">
         <f t="shared" si="0"/>
         <v>135296</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="20">
         <f t="shared" si="0"/>
         <v>270592</v>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="25">
         <f t="shared" si="0"/>
         <v>541184</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="2" t="str">
-        <f>CONCATENATE(J3, " , ", K3, " , ", L3, " , ", M3, " , ", N3)</f>
-        <v>33824 , 67648 , 135296 , 270592 , 541184</v>
+        <f>CONCATENATE(J3, ",", K3, ",", L3, ",", M3, ",", N3)</f>
+        <v>33824,67648,135296,270592,541184</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="35">
+      <c r="C4" s="34">
         <f t="shared" ref="C4:C6" si="3">G3*2</f>
         <v>1024</v>
       </c>
@@ -1304,37 +1291,37 @@
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="26">
         <f t="shared" si="2"/>
         <v>1082368</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <f t="shared" si="0"/>
         <v>2164736</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="8">
         <f t="shared" si="0"/>
         <v>4329472</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="8">
         <f t="shared" si="0"/>
         <v>8658944</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="23">
         <f t="shared" si="0"/>
         <v>17317888</v>
       </c>
       <c r="Q4" s="2" t="str">
-        <f>CONCATENATE(J4, " , ", K4, " , ", L4, " , ", M4, " , ", N4)</f>
-        <v>1082368 , 2164736 , 4329472 , 8658944 , 17317888</v>
+        <f>CONCATENATE(J4, ",", K4, ",", L4, ",", M4, ",", N4)</f>
+        <v>1082368,2164736,4329472,8658944,17317888</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="35">
+      <c r="C5" s="34">
         <f t="shared" si="3"/>
         <v>32768</v>
       </c>
@@ -1350,220 +1337,221 @@
         <f t="shared" si="1"/>
         <v>262144</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <f t="shared" si="1"/>
         <v>524288</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <f t="shared" si="3"/>
         <v>1048576</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <f t="shared" si="1"/>
         <v>2097152</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <f t="shared" si="1"/>
         <v>4194304</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="18">
         <f t="shared" si="1"/>
         <v>8388608</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="19">
         <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="21">
         <f>C2+D2+E2</f>
         <v>7</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="22">
         <f>D2+E2+F2</f>
         <v>14</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="27">
         <f>E2+F2+G2</f>
         <v>28</v>
       </c>
       <c r="Q6" s="2" t="str">
-        <f>CONCATENATE(L6, " , ", L7, " , ", L8, " , ", L9, " , ", L10)</f>
-        <v>7 , 224 , 7168 , 229376 , 7340032</v>
+        <f>CONCATENATE(L6, ",", L7, ",", L8, ",", L9, ",", L10)</f>
+        <v>7,224,7168,229376,7340032</v>
       </c>
       <c r="R6" s="2" t="str">
-        <f>CONCATENATE(M6, " , ", M7, " , ", M8, " , ", M9, " , ", M10)</f>
-        <v>14 , 448 , 14336 , 458752 , 14680064</v>
+        <f>CONCATENATE(M6, ",", M7, ",", M8, ",", M9, ",", M10)</f>
+        <v>14,448,14336,458752,14680064</v>
       </c>
       <c r="S6" s="2" t="str">
-        <f>CONCATENATE(N6, " , ", N7, " , ", N8, " , ", N9, " , ", N10)</f>
-        <v>28 , 896 , 28672 , 917504 , 29360128</v>
+        <f>CONCATENATE(N6, ",", N7, ",", N8, ",", N9, ",", N10)</f>
+        <v>28,896,28672,917504,29360128</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L7" s="25">
+      <c r="L7" s="24">
         <f>C3+D3+E3</f>
         <v>224</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="20">
         <f>D3+E3+F3</f>
         <v>448</v>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="25">
         <f>E3+F3+G3</f>
         <v>896</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <f>C2+D3+E4</f>
         <v>4161</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <f t="shared" ref="D8:E10" si="4">D2+E3+F4</f>
         <v>8322</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <f t="shared" si="4"/>
         <v>16644</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <f>C4+D3+E2</f>
         <v>1092</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <f>D4+E3+F2</f>
         <v>2184</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="11">
         <f>E4+F3+G2</f>
         <v>4368</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="24">
         <f>C4+D4+E4</f>
         <v>7168</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="20">
         <f>D4+E4+F4</f>
         <v>14336</v>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="25">
         <f>E4+F4+G4</f>
         <v>28672</v>
       </c>
       <c r="Q8" s="2" t="str">
-        <f>CONCATENATE(C8, " , ", D8, " , ", E8, " , ", C9, " , ", D9, " , ", E9, " , ", C10, " , ", D10, " , ", E10)</f>
-        <v>4161 , 8322 , 16644 , 133152 , 266304 , 532608 , 4260864 , 8521728 , 17043456</v>
+        <f>CONCATENATE(C8, ",", D8, ",", E8, ",", C9, ",", D9, ",", E9, ",", C10, ",", D10, ",", E10)</f>
+        <v>4161,8322,16644,133152,266304,532608,4260864,8521728,17043456</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <f t="shared" ref="C9:C10" si="5">C3+D4+E5</f>
         <v>133152</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <f t="shared" si="4"/>
         <v>266304</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="25">
         <f>E3+F4+G5</f>
         <v>532608</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="24">
         <f>C5+D4+E3</f>
         <v>34944</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <f>D5+E4+F3</f>
         <v>69888</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="25">
         <f>E5+F4+G3</f>
         <v>139776</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="24">
         <f>C5+D5+E5</f>
         <v>229376</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="20">
         <f>D5+E5+F5</f>
         <v>458752</v>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="25">
         <f>E5+F5+G5</f>
         <v>917504</v>
       </c>
       <c r="Q9" s="2" t="str">
-        <f>CONCATENATE(H8, " , ", I8, " , ", J8, " , ", H9, " , ", I9, " , ", J9, " , ", I10, " , ", J10)</f>
-        <v>1092 , 2184 , 4368 , 34944 , 69888 , 139776 , 2236416 , 4472832</v>
+        <f>CONCATENATE(H8, ",", I8, ",", J8, ",", H9, ",", I9, ",", J9, ",", I10, ",", J10)</f>
+        <v>1092,2184,4368,34944,69888,139776,2236416,4472832</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <f t="shared" si="5"/>
         <v>4260864</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <f t="shared" si="4"/>
         <v>8521728</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="23">
         <f t="shared" si="4"/>
         <v>17043456</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f>C6+D5+E4</f>
         <v>1118208</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <f>D6+E5+F4</f>
         <v>2236416</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="30">
         <f>E6+F5+G4</f>
         <v>4472832</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="7">
         <f>C6+D6+E6</f>
         <v>7340032</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="8">
         <f>D6+E6+F6</f>
         <v>14680064</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="23">
         <f>E6+F6+G6</f>
         <v>29360128</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="121" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q11" s="39" t="str">
-        <f>CONCATENATE(Q2, " , ", Q3, " , ", Q4, " , ", Q6, " , ", R6, " , ", S6, " , ", Q8, " , ", Q9)</f>
-        <v>1057 , 2114 , 4228 , 8456 , 16912 , 33824 , 67648 , 135296 , 270592 , 541184 , 1082368 , 2164736 , 4329472 , 8658944 , 17317888 , 7 , 224 , 7168 , 229376 , 7340032 , 14 , 448 , 14336 , 458752 , 14680064 , 28 , 896 , 28672 , 917504 , 29360128 , 4161 , 8322 , 16644 , 133152 , 266304 , 532608 , 4260864 , 8521728 , 17043456 , 1092 , 2184 , 4368 , 34944 , 69888 , 139776 , 2236416 , 4472832</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" ht="121" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="5" t="s">
+      <c r="P11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="38" t="str">
+        <f>CONCATENATE(Q2, ",", Q3, ",", Q4, ",", Q6, ",", R6, ",", S6, ",", Q8, ",", Q9)</f>
+        <v>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="40" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="P2:S12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
>>app.js: added in some large text to make sections easier to find on the minimap, will delete later. corrected various css bugs. amended row 92 in createRowValues to match values in the Excel file. Added more information about Bitwise checking. Removed welcomeBanner2. Added an 'enableClick' class when columns are first initiated. Amended lots of styling rows 240 thru to 282. Line 324-5 juggled some classes when click happens. Built in the 'reset css' styling.
</commit_message>
<xml_diff>
--- a/resources/calculate_winningScores.xlsx
+++ b/resources/calculate_winningScores.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t>vert:</t>
   </si>
@@ -65,13 +65,57 @@
   </si>
   <si>
     <t>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832</t>
+  </si>
+  <si>
+    <t>273,84,73,146,292,7,56,448</t>
+  </si>
+  <si>
+    <t>273,546,1092,2184,4368,8736,17472,34944,7,14,112,224,1792,3584,28672,57344</t>
+  </si>
+  <si>
+    <t>G4L3
+Text format:</t>
+  </si>
+  <si>
+    <t>3-in-a-row</t>
+  </si>
+  <si>
+    <t>4-in-a-row</t>
+  </si>
+  <si>
+    <t>vert</t>
+  </si>
+  <si>
+    <t>33825,4680,4369,8738,17476,34952,15,240,3840,61440</t>
+  </si>
+  <si>
+    <t>G4L4
+Text format:</t>
+  </si>
+  <si>
+    <t>G5L3</t>
+  </si>
+  <si>
+    <t>G5L4</t>
+  </si>
+  <si>
+    <t>266305,532610,8521760,17043520,34952,69904,1118464,2236928,33825,67650,135300,270600,541200,1082400,2164800,4329600,8659200,17318400,15,30,480,960,15360,30720,491520,983040,15728640,31457280</t>
+  </si>
+  <si>
+    <t>5-in-a-row</t>
+  </si>
+  <si>
+    <t>17043521,1118480,1082401,2164802,4329604,8659208,17318416,31,992,31744,1015808,32505856</t>
+  </si>
+  <si>
+    <t>G5L5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,8 +137,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +176,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -150,6 +213,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -429,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,12 +513,141 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,100 +657,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -830,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J7"/>
+  <dimension ref="B1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -838,32 +968,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.5" style="1"/>
+    <col min="1" max="11" width="9.5" style="1"/>
+    <col min="12" max="12" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12">
+    <row r="1" spans="2:13" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="14">
         <f>B2*2</f>
         <v>2</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="15">
         <f>C2*2</f>
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="7">
         <f>B2+C3+D4</f>
         <v>273</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="15">
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f>CONCATENATE(H2,",",H3,",",H4,",",I4,",",J4,",",H5,",",H6,",",H7)</f>
+        <v>273,84,73,146,292,7,56,448</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
         <f>D2*2</f>
         <v>8</v>
       </c>
@@ -871,64 +1011,74 @@
         <f>B3*2</f>
         <v>16</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="17">
         <f>C3*2</f>
         <v>32</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="7">
         <f>B4+C3+D2</f>
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
         <f>D3*2</f>
         <v>64</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="19">
         <f>B4*2</f>
         <v>128</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="20">
         <f>C4*2</f>
         <v>256</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="9">
         <f>B2+B3+B4</f>
         <v>73</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <f>C2+C3+C4</f>
         <v>146</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="7">
         <f>D2+D3+D4</f>
         <v>292</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="2" t="s">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="12">
         <f>B2+C2+D2</f>
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H6" s="9">
+    <row r="6" spans="2:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="10">
         <f>B3+C3+D3</f>
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H7" s="10">
+    <row r="7" spans="2:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="11">
         <f>B4+C4+D4</f>
         <v>448</v>
       </c>
@@ -941,67 +1091,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O7"/>
+  <dimension ref="B1:X13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.5" style="1"/>
+    <col min="1" max="12" width="9.5" style="1"/>
+    <col min="13" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.5" style="1"/>
+    <col min="17" max="17" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" style="1"/>
+    <col min="20" max="20" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="103.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12">
+    <row r="1" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+    </row>
+    <row r="2" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="14">
         <f>B2*2</f>
         <v>2</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <f>C2*2</f>
         <v>4</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="15">
         <f>D2*2</f>
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <f>B2+C3+D4</f>
         <v>1057</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="26">
         <f>C2+D3+E4</f>
         <v>2114</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="21">
+      <c r="L2" s="25">
         <f>B2+B3+B4</f>
         <v>273</v>
       </c>
-      <c r="M2" s="22">
+      <c r="M2" s="21">
         <f t="shared" ref="M2:O2" si="0">C2+C3+C4</f>
         <v>546</v>
       </c>
-      <c r="N2" s="22">
+      <c r="N2" s="21">
         <f t="shared" si="0"/>
         <v>1092</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="26">
         <f t="shared" si="0"/>
         <v>2184</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="15">
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <f>CONCATENATE(L2,",",M2,",",N2,",",O2)</f>
+        <v>273,546,1092,2184</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="1" t="str">
+        <f>CONCATENATE(R2,",",R3,",",R4,",",R5,",",R6,",",R7)</f>
+        <v>273,546,1092,2184,4368,8736,17472,34944,7,14,112,224,1792,3584,28672,57344</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
         <f>E2*2</f>
         <v>16</v>
       </c>
@@ -1013,38 +1208,51 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="17">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="7">
+      <c r="G3" s="21"/>
+      <c r="H3" s="8">
         <f>B3+C4+D5</f>
         <v>16912</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="24">
         <f>C3+D4+E5</f>
         <v>33824</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="25">
         <f>B3+B4+B5</f>
         <v>4368</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="21">
         <f t="shared" ref="M3" si="2">C3+C4+C5</f>
         <v>8736</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="9">
         <f t="shared" ref="N3" si="3">D3+D4+D5</f>
         <v>17472</v>
       </c>
-      <c r="O3" s="23">
+      <c r="O3" s="24">
         <f t="shared" ref="O3" si="4">E3+E4+E5</f>
         <v>34944</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="15">
+      <c r="Q3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <f>CONCATENATE(L3,",",M3,",",N3,",",O3)</f>
+        <v>4368,8736,17472,34944</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="16">
         <f t="shared" ref="B4:B5" si="5">E3*2</f>
         <v>256</v>
       </c>
@@ -1056,102 +1264,223 @@
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="17">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="23">
         <f>B4+C3+D2</f>
         <v>292</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="12">
         <f>C4+D3+E2</f>
         <v>584</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="22">
         <f>B2+C2+D2</f>
         <v>7</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="12">
         <f>C2+D2+E2</f>
         <v>14</v>
       </c>
-      <c r="N4" s="20"/>
-    </row>
-    <row r="5" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
+      <c r="N4" s="21"/>
+      <c r="R4" s="1" t="str">
+        <f>CONCATENATE(L4,",",M4)</f>
+        <v>7,14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
         <f t="shared" si="5"/>
         <v>4096</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="19">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="19">
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="20">
         <f t="shared" si="1"/>
         <v>32768</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="8">
         <f>B5+C4+D3</f>
         <v>4672</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="24">
         <f>C5+D4+E3</f>
         <v>9344</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="24">
+      <c r="K5" s="21"/>
+      <c r="L5" s="25">
         <f>B3+C3+D3</f>
         <v>112</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="26">
         <f>C3+D3+E3</f>
         <v>224</v>
       </c>
-      <c r="N5" s="20"/>
-    </row>
-    <row r="6" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K6" s="20"/>
-      <c r="L6" s="24">
+      <c r="N5" s="21"/>
+      <c r="R5" s="1" t="str">
+        <f t="shared" ref="R5:R7" si="6">CONCATENATE(L5,",",M5)</f>
+        <v>112,224</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="21"/>
+      <c r="L6" s="25">
         <f>B4+C4+D4</f>
         <v>1792</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="26">
         <f>C4+D4+E4</f>
         <v>3584</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L7" s="7">
+      <c r="R6" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>1792,3584</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="25">
         <f>B5+C5+D5</f>
         <v>28672</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="26">
         <f>C5+D5+E5</f>
         <v>57344</v>
       </c>
+      <c r="R7" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>28672,57344</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G8" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+      <c r="X8" s="44"/>
+    </row>
+    <row r="9" spans="2:24" ht="73" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="11">
+        <f>B2+C3+D4+E5</f>
+        <v>33825</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="11">
+        <f>B2+B3+B4+B5</f>
+        <v>4369</v>
+      </c>
+      <c r="L9" s="11">
+        <f t="shared" ref="L9:N9" si="7">C2+C3+C4+C5</f>
+        <v>8738</v>
+      </c>
+      <c r="M9" s="11">
+        <f t="shared" si="7"/>
+        <v>17476</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="7"/>
+        <v>34952</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="3" t="str">
+        <f>CONCATENATE(H9,",",H10,",",K9,",",L9,",",M9,",",N9,",",K10,",",K11,",",K12,",",K13)</f>
+        <v>33825,4680,4369,8738,17476,34952,15,240,3840,61440</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" ht="73" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <f>B5+C4+D3+E2</f>
+        <v>4680</v>
+      </c>
+      <c r="J10" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11">
+        <f>B2+C2+D2+E2</f>
+        <v>15</v>
+      </c>
+      <c r="Q10" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="2">
+        <f>B3+C3+D3+E3</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="2">
+        <f>B4+C4+D4+E4</f>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="2">
+        <f>B5+C5+D5+E5</f>
+        <v>61440</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="G8:O8"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="P1:X1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S12"/>
+  <dimension ref="B1:X31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J8" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1159,26 +1488,34 @@
     <col min="1" max="1" width="9.5" style="1"/>
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.5" style="1"/>
-    <col min="10" max="10" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" style="1"/>
     <col min="16" max="16" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="110" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="110" style="38" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="48.5" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="12">
+    <row r="1" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="50"/>
+    </row>
+    <row r="2" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <f>C2*2</f>
         <v>2</v>
       </c>
@@ -1194,92 +1531,92 @@
         <f>F2*2</f>
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="21">
+      <c r="J2" s="22">
         <f>C2+C3+C4</f>
         <v>1057</v>
       </c>
-      <c r="K2" s="22">
+      <c r="K2" s="23">
         <f t="shared" ref="K2:N4" si="0">D2+D3+D4</f>
         <v>2114</v>
       </c>
-      <c r="L2" s="22">
+      <c r="L2" s="23">
         <f t="shared" si="0"/>
         <v>4228</v>
       </c>
-      <c r="M2" s="22">
+      <c r="M2" s="23">
         <f t="shared" si="0"/>
         <v>8456</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="12">
         <f t="shared" si="0"/>
         <v>16912</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="2" t="str">
+      <c r="Q2" s="56" t="str">
         <f>CONCATENATE(J2, ",", K2, ",", L2, ",", M2, ",", N2)</f>
         <v>1057,2114,4228,8456,16912</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="33">
         <f>G2*2</f>
         <v>32</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="52">
         <f t="shared" ref="D3:G6" si="1">C3*2</f>
         <v>64</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="52">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="52">
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="53">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="25">
         <f t="shared" ref="J3:J4" si="2">C3+C4+C5</f>
         <v>33824</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="21">
         <f t="shared" si="0"/>
         <v>67648</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="21">
         <f t="shared" si="0"/>
         <v>135296</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="21">
         <f t="shared" si="0"/>
         <v>270592</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="26">
         <f t="shared" si="0"/>
         <v>541184</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="2" t="str">
+      <c r="Q3" s="56" t="str">
         <f>CONCATENATE(J3, ",", K3, ",", L3, ",", M3, ",", N3)</f>
         <v>33824,67648,135296,270592,541184</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="34">
         <f t="shared" ref="C4:C6" si="3">G3*2</f>
         <v>1024</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
@@ -1295,32 +1632,32 @@
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="27">
         <f t="shared" si="2"/>
         <v>1082368</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="9">
         <f t="shared" si="0"/>
         <v>2164736</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="9">
         <f t="shared" si="0"/>
         <v>4329472</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
         <v>8658944</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="24">
         <f t="shared" si="0"/>
         <v>17317888</v>
       </c>
-      <c r="Q4" s="2" t="str">
+      <c r="Q4" s="56" t="str">
         <f>CONCATENATE(J4, ",", K4, ",", L4, ",", M4, ",", N4)</f>
         <v>1082368,2164736,4329472,8658944,17317888</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="34">
         <f t="shared" si="3"/>
         <v>32768</v>
@@ -1329,25 +1666,25 @@
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>131072</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
         <v>262144</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="17">
         <f t="shared" si="1"/>
         <v>524288</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="36">
         <f t="shared" si="3"/>
         <v>1048576</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="19">
         <f t="shared" si="1"/>
         <v>2097152</v>
       </c>
@@ -1355,30 +1692,30 @@
         <f t="shared" si="1"/>
         <v>4194304</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="19">
         <f t="shared" si="1"/>
         <v>8388608</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="20">
         <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="22">
         <f>C2+D2+E2</f>
         <v>7</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="23">
         <f>D2+E2+F2</f>
         <v>14</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="28">
         <f>E2+F2+G2</f>
         <v>28</v>
       </c>
-      <c r="Q6" s="2" t="str">
+      <c r="Q6" s="56" t="str">
         <f>CONCATENATE(L6, ",", L7, ",", L8, ",", L9, ",", L10)</f>
         <v>7,224,7168,229376,7340032</v>
       </c>
@@ -1391,128 +1728,128 @@
         <v>28,896,28672,917504,29360128</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L7" s="24">
+    <row r="7" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="25">
         <f>C3+D3+E3</f>
         <v>224</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="21">
         <f>D3+E3+F3</f>
         <v>448</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="26">
         <f>E3+F3+G3</f>
         <v>896</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
+    <row r="8" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="22">
         <f>C2+D3+E4</f>
         <v>4161</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="23">
         <f t="shared" ref="D8:E10" si="4">D2+E3+F4</f>
         <v>8322</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="12">
         <f t="shared" si="4"/>
         <v>16644</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="22">
         <f>C4+D3+E2</f>
         <v>1092</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="23">
         <f>D4+E3+F2</f>
         <v>2184</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="12">
         <f>E4+F3+G2</f>
         <v>4368</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="25">
         <f>C4+D4+E4</f>
         <v>7168</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="21">
         <f>D4+E4+F4</f>
         <v>14336</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="26">
         <f>E4+F4+G4</f>
         <v>28672</v>
       </c>
-      <c r="Q8" s="2" t="str">
+      <c r="Q8" s="56" t="str">
         <f>CONCATENATE(C8, ",", D8, ",", E8, ",", C9, ",", D9, ",", E9, ",", C10, ",", D10, ",", E10)</f>
         <v>4161,8322,16644,133152,266304,532608,4260864,8521728,17043456</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="28">
+    <row r="9" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="29">
         <f t="shared" ref="C9:C10" si="5">C3+D4+E5</f>
         <v>133152</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="21">
         <f t="shared" si="4"/>
         <v>266304</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="26">
         <f>E3+F4+G5</f>
         <v>532608</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="25">
         <f>C5+D4+E3</f>
         <v>34944</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="21">
         <f>D5+E4+F3</f>
         <v>69888</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="26">
         <f>E5+F4+G3</f>
         <v>139776</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="25">
         <f>C5+D5+E5</f>
         <v>229376</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="21">
         <f>D5+E5+F5</f>
         <v>458752</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="26">
         <f>E5+F5+G5</f>
         <v>917504</v>
       </c>
-      <c r="Q9" s="2" t="str">
+      <c r="Q9" s="56" t="str">
         <f>CONCATENATE(H8, ",", I8, ",", J8, ",", H9, ",", I9, ",", J9, ",", I10, ",", J10)</f>
         <v>1092,2184,4368,34944,69888,139776,2236416,4472832</v>
       </c>
     </row>
-    <row r="10" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="7">
+    <row r="10" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="8">
         <f t="shared" si="5"/>
         <v>4260864</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <f t="shared" si="4"/>
         <v>8521728</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="24">
         <f t="shared" si="4"/>
         <v>17043456</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="8">
         <f>C6+D5+E4</f>
         <v>1118208</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="9">
         <f>D6+E5+F4</f>
         <v>2236416</v>
       </c>
@@ -1520,38 +1857,353 @@
         <f>E6+F5+G4</f>
         <v>4472832</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="8">
         <f>C6+D6+E6</f>
         <v>7340032</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="9">
         <f>D6+E6+F6</f>
         <v>14680064</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="24">
         <f>E6+F6+G6</f>
         <v>29360128</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="121" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P11" s="20" t="s">
+    <row r="11" spans="2:24" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="38" t="str">
+      <c r="Q11" s="40" t="str">
         <f>CONCATENATE(Q2, ",", Q3, ",", Q4, ",", Q6, ",", R6, ",", S6, ",", Q8, ",", Q9)</f>
         <v>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832</v>
       </c>
     </row>
-    <row r="12" spans="2:19" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q12" s="39" t="s">
+    <row r="12" spans="2:24" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="41" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="55"/>
+      <c r="V14" s="55"/>
+      <c r="W14" s="55"/>
+      <c r="X14" s="55"/>
+    </row>
+    <row r="15" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11">
+        <f>C2+D3+E4+F5</f>
+        <v>266305</v>
+      </c>
+      <c r="E15" s="11">
+        <f>D2+E3+F4+G5</f>
+        <v>532610</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="11">
+        <f>C2+C3+C4+C5</f>
+        <v>33825</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" ref="J15:L15" si="6">D2+D3+D4+D5</f>
+        <v>67650</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="6"/>
+        <v>135300</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="6"/>
+        <v>270600</v>
+      </c>
+      <c r="M15" s="11">
+        <f>G2+G3+G4+G5</f>
+        <v>541200</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="38" t="str">
+        <f>CONCATENATE(D15,",",E15,",",D16,",",E16,",",D17,",",E17,",",D18,",",E18)</f>
+        <v>266305,532610,8521760,17043520,34952,69904,1118464,2236928</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="11">
+        <f>C3+D4+E5+F6</f>
+        <v>8521760</v>
+      </c>
+      <c r="E16" s="11">
+        <f>D3+E4+F5+G6</f>
+        <v>17043520</v>
+      </c>
+      <c r="I16" s="11">
+        <f>C3+C4+C5+C6</f>
+        <v>1082400</v>
+      </c>
+      <c r="J16" s="11">
+        <f t="shared" ref="J16" si="7">D3+D4+D5+D6</f>
+        <v>2164800</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" ref="K16" si="8">E3+E4+E5+E6</f>
+        <v>4329600</v>
+      </c>
+      <c r="L16" s="11">
+        <f t="shared" ref="L16" si="9">F3+F4+F5+F6</f>
+        <v>8659200</v>
+      </c>
+      <c r="M16" s="11">
+        <f>G3+G4+G5+G6</f>
+        <v>17318400</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="39" t="str">
+        <f>CONCATENATE(I15,",",J15,",",K15,",",L15,",",M15,",",I16,",",J16,",",K16,",",L16,",",M16)</f>
+        <v>33825,67650,135300,270600,541200,1082400,2164800,4329600,8659200,17318400</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <f>C5+D4+E3+F2</f>
+        <v>34952</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D5+E4+F3+G2</f>
+        <v>69904</v>
+      </c>
+      <c r="H17" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="11">
+        <f>C2+D2+E2+F2</f>
+        <v>15</v>
+      </c>
+      <c r="J17" s="11">
+        <f>D2+E2+F2+G2</f>
+        <v>30</v>
+      </c>
+      <c r="Q17" s="38" t="str">
+        <f>CONCATENATE(I17,",",J17,",",I18,",",J18,",",I19,",",J19,",",I20,",",J20,",",I21,",",J21)</f>
+        <v>15,30,480,960,15360,30720,491520,983040,15728640,31457280</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="2">
+        <f>C6+D5+E4+F3</f>
+        <v>1118464</v>
+      </c>
+      <c r="E18" s="2">
+        <f>D6+E5+F4+G3</f>
+        <v>2236928</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" ref="I18:J18" si="10">C3+D3+E3+F3</f>
+        <v>480</v>
+      </c>
+      <c r="J18" s="54">
+        <f t="shared" si="10"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" ht="73" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="11">
+        <f t="shared" ref="I19:J19" si="11">C4+D4+E4+F4</f>
+        <v>15360</v>
+      </c>
+      <c r="J19" s="11">
+        <f t="shared" si="11"/>
+        <v>30720</v>
+      </c>
+      <c r="P19" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="57" t="str">
+        <f>CONCATENATE(Q15,",",Q16,",",Q17)</f>
+        <v>266305,532610,8521760,17043520,34952,69904,1118464,2236928,33825,67650,135300,270600,541200,1082400,2164800,4329600,8659200,17318400,15,30,480,960,15360,30720,491520,983040,15728640,31457280</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" ht="73" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="11">
+        <f t="shared" ref="I20:J20" si="12">C5+D5+E5+F5</f>
+        <v>491520</v>
+      </c>
+      <c r="J20" s="11">
+        <f t="shared" si="12"/>
+        <v>983040</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="11">
+        <f t="shared" ref="I21:J21" si="13">C6+D6+E6+F6</f>
+        <v>15728640</v>
+      </c>
+      <c r="J21" s="11">
+        <f t="shared" si="13"/>
+        <v>31457280</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="50"/>
+    </row>
+    <row r="24" spans="3:17" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="24">
+        <f>C2+D3+E4+F5+G6</f>
+        <v>17043521</v>
+      </c>
+      <c r="P24" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="57" t="str">
+        <f>CONCATENATE(D24,",",D25,",",D26,",",E26,",",F26,",",G26,",",H26,",",D27,",",D28,",",D29,",",D30,",",D31)</f>
+        <v>17043521,1118480,1082401,2164802,4329604,8659208,17318416,31,992,31744,1015808,32505856</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7">
+        <f>C6+D5+E4+F3+G2</f>
+        <v>1118480</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="P25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <f>C2+C3+C4+C5+C6</f>
+        <v>1082401</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" ref="E26:H26" si="14">D2+D3+D4+D5+D6</f>
+        <v>2164802</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="14"/>
+        <v>4329604</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="14"/>
+        <v>8659208</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="14"/>
+        <v>17318416</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <f>C2+D2+E2+F2+G2</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28" s="2">
+        <f t="shared" ref="D28:D31" si="15">C3+D3+E3+F3+G3</f>
+        <v>992</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="2">
+        <f t="shared" si="15"/>
+        <v>31744</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="2">
+        <f t="shared" si="15"/>
+        <v>1015808</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="2">
+        <f t="shared" si="15"/>
+        <v>32505856</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="P2:S12"/>
+  <mergeCells count="5">
+    <mergeCell ref="C23:L23"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="C14:M14"/>
+    <mergeCell ref="N14:R14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated file for PDF output
</commit_message>
<xml_diff>
--- a/resources/calculate_winningScores.xlsx
+++ b/resources/calculate_winningScores.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noccer/Dropbox/Niall/WDI-7/03_Week/resources/"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'5x5'!$P$2:$S$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'5x5'!$A$1:$S$31</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -64,13 +65,7 @@
     <t>Text format:</t>
   </si>
   <si>
-    <t>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832</t>
-  </si>
-  <si>
     <t>273,84,73,146,292,7,56,448</t>
-  </si>
-  <si>
-    <t>273,546,1092,2184,4368,8736,17472,34944,7,14,112,224,1792,3584,28672,57344</t>
   </si>
   <si>
     <t>G4L3
@@ -109,13 +104,19 @@
   </si>
   <si>
     <t>G5L5</t>
+  </si>
+  <si>
+    <t>273,546,1092,2184,4368,8736,17472,34944,7,14,112,224,1792,3584,28672,573441057,2114,16912,33824,292,584,4672,9344</t>
+  </si>
+  <si>
+    <t>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832,1118208</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +143,28 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -502,10 +525,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -636,9 +661,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -648,15 +670,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -678,8 +691,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -980,14 +1022,14 @@
         <v>1</v>
       </c>
       <c r="C2" s="14">
-        <f>B2*2</f>
+        <f t="shared" ref="C2:D4" si="0">B2*2</f>
         <v>2</v>
       </c>
       <c r="D2" s="15">
-        <f>C2*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="45" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="7">
@@ -1008,14 +1050,14 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <f>B3*2</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D3" s="17">
-        <f>C3*2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="45" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="7">
@@ -1032,14 +1074,14 @@
         <v>64</v>
       </c>
       <c r="C4" s="19">
-        <f>B4*2</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="D4" s="20">
-        <f>C4*2</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="44" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="9">
@@ -1059,11 +1101,11 @@
         <v>9</v>
       </c>
       <c r="M4" s="42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="12">
@@ -1093,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1111,28 +1153,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
+      <c r="G1" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
     </row>
     <row r="2" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13">
@@ -1150,7 +1192,7 @@
         <f>D2*2</f>
         <v>8</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="21">
@@ -1161,7 +1203,7 @@
         <f>C2+D3+E4</f>
         <v>2114</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="44" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="25">
@@ -1183,17 +1225,20 @@
       <c r="Q2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1" t="str">
+      <c r="R2" s="2" t="str">
         <f>CONCATENATE(L2,",",M2,",",N2,",",O2)</f>
         <v>273,546,1092,2184</v>
       </c>
       <c r="T2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="1" t="str">
-        <f>CONCATENATE(R2,",",R3,",",R4,",",R5,",",R6,",",R7)</f>
-        <v>273,546,1092,2184,4368,8736,17472,34944,7,14,112,224,1792,3584,28672,57344</v>
-      </c>
+      <c r="U2" s="59" t="str">
+        <f>CONCATENATE(R2,",",R3,",",R4,",",R5,",",R6,",",R7,Q4)</f>
+        <v>273,546,1092,2184,4368,8736,17472,34944,7,14,112,224,1792,3584,28672,573441057,2114,16912,33824,292,584,4672,9344</v>
+      </c>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
     </row>
     <row r="3" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16">
@@ -1240,18 +1285,18 @@
       <c r="Q3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="1" t="str">
+      <c r="R3" s="2" t="str">
         <f>CONCATENATE(L3,",",M3,",",N3,",",O3)</f>
         <v>4368,8736,17472,34944</v>
       </c>
       <c r="T3" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" s="42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="U3" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="96" x14ac:dyDescent="0.2">
       <c r="B4" s="16">
         <f t="shared" ref="B4:B5" si="5">E3*2</f>
         <v>256</v>
@@ -1268,7 +1313,7 @@
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="45" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="23">
@@ -1279,19 +1324,23 @@
         <f>C4+D3+E2</f>
         <v>584</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="45" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="22">
-        <f>B2+C2+D2</f>
+        <f t="shared" ref="L4:M7" si="6">B2+C2+D2</f>
         <v>7</v>
       </c>
       <c r="M4" s="12">
-        <f>C2+D2+E2</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="N4" s="21"/>
-      <c r="R4" s="1" t="str">
+      <c r="Q4" s="60" t="str">
+        <f>CONCATENATE(H2,",",I2,",",H3,",",I3,",",H4,",",I4,",",H5,",",I5)</f>
+        <v>1057,2114,16912,33824,292,584,4672,9344</v>
+      </c>
+      <c r="R4" s="2" t="str">
         <f>CONCATENATE(L4,",",M4)</f>
         <v>7,14</v>
       </c>
@@ -1323,97 +1372,97 @@
       </c>
       <c r="K5" s="21"/>
       <c r="L5" s="25">
-        <f>B3+C3+D3</f>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="M5" s="26">
-        <f>C3+D3+E3</f>
+        <f t="shared" si="6"/>
         <v>224</v>
       </c>
       <c r="N5" s="21"/>
-      <c r="R5" s="1" t="str">
-        <f t="shared" ref="R5:R7" si="6">CONCATENATE(L5,",",M5)</f>
+      <c r="R5" s="2" t="str">
+        <f t="shared" ref="R5:R7" si="7">CONCATENATE(L5,",",M5)</f>
         <v>112,224</v>
       </c>
     </row>
     <row r="6" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K6" s="21"/>
       <c r="L6" s="25">
-        <f>B4+C4+D4</f>
+        <f t="shared" si="6"/>
         <v>1792</v>
       </c>
       <c r="M6" s="26">
-        <f>C4+D4+E4</f>
+        <f t="shared" si="6"/>
         <v>3584</v>
       </c>
-      <c r="R6" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="R6" s="2" t="str">
+        <f t="shared" si="7"/>
         <v>1792,3584</v>
       </c>
     </row>
     <row r="7" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L7" s="25">
-        <f>B5+C5+D5</f>
+        <f t="shared" si="6"/>
         <v>28672</v>
       </c>
       <c r="M7" s="26">
-        <f>C5+D5+E5</f>
+        <f t="shared" si="6"/>
         <v>57344</v>
       </c>
-      <c r="R7" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="R7" s="2" t="str">
+        <f t="shared" si="7"/>
         <v>28672,57344</v>
       </c>
     </row>
     <row r="8" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="44"/>
-      <c r="U8" s="44"/>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
-      <c r="X8" s="44"/>
+      <c r="G8" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
     </row>
     <row r="9" spans="2:24" ht="73" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="44" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="11">
         <f>B2+C3+D4+E5</f>
         <v>33825</v>
       </c>
-      <c r="J9" s="45" t="s">
-        <v>16</v>
+      <c r="J9" s="44" t="s">
+        <v>14</v>
       </c>
       <c r="K9" s="11">
         <f>B2+B3+B4+B5</f>
         <v>4369</v>
       </c>
       <c r="L9" s="11">
-        <f t="shared" ref="L9:N9" si="7">C2+C3+C4+C5</f>
+        <f t="shared" ref="L9:N9" si="8">C2+C3+C4+C5</f>
         <v>8738</v>
       </c>
       <c r="M9" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17476</v>
       </c>
       <c r="N9" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>34952</v>
       </c>
       <c r="Q9" s="21" t="s">
@@ -1425,14 +1474,14 @@
       </c>
     </row>
     <row r="10" spans="2:24" ht="73" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="45" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="2">
         <f>B5+C4+D3+E2</f>
         <v>4680</v>
       </c>
-      <c r="J10" s="46" t="s">
+      <c r="J10" s="45" t="s">
         <v>1</v>
       </c>
       <c r="K10" s="11">
@@ -1440,10 +1489,10 @@
         <v>15</v>
       </c>
       <c r="Q10" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="R10" s="47" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="R10" s="46" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -1477,10 +1526,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:X31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="25" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="S1" sqref="A1:S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="57" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1502,14 +1554,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I1" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="50"/>
+      <c r="I1" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="13">
@@ -1531,7 +1583,7 @@
         <f>F2*2</f>
         <v>16</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="45" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="22">
@@ -1557,7 +1609,7 @@
       <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="56" t="str">
+      <c r="Q2" s="52" t="str">
         <f>CONCATENATE(J2, ",", K2, ",", L2, ",", M2, ",", N2)</f>
         <v>1057,2114,4228,8456,16912</v>
       </c>
@@ -1567,19 +1619,19 @@
         <f>G2*2</f>
         <v>32</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="48">
         <f t="shared" ref="D3:G6" si="1">C3*2</f>
         <v>64</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="48">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="48">
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="49">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
@@ -1606,7 +1658,7 @@
       <c r="P3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="56" t="str">
+      <c r="Q3" s="52" t="str">
         <f>CONCATENATE(J3, ",", K3, ",", L3, ",", M3, ",", N3)</f>
         <v>33824,67648,135296,270592,541184</v>
       </c>
@@ -1652,7 +1704,7 @@
         <f t="shared" si="0"/>
         <v>17317888</v>
       </c>
-      <c r="Q4" s="56" t="str">
+      <c r="Q4" s="52" t="str">
         <f>CONCATENATE(J4, ",", K4, ",", L4, ",", M4, ",", N4)</f>
         <v>1082368,2164736,4329472,8658944,17317888</v>
       </c>
@@ -1700,22 +1752,22 @@
         <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
-      <c r="K6" s="46" t="s">
+      <c r="K6" s="45" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="22">
-        <f>C2+D2+E2</f>
+        <f t="shared" ref="L6:N10" si="4">C2+D2+E2</f>
         <v>7</v>
       </c>
       <c r="M6" s="23">
-        <f>D2+E2+F2</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="N6" s="28">
-        <f>E2+F2+G2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="Q6" s="56" t="str">
+      <c r="Q6" s="52" t="str">
         <f>CONCATENATE(L6, ",", L7, ",", L8, ",", L9, ",", L10)</f>
         <v>7,224,7168,229376,7340032</v>
       </c>
@@ -1730,20 +1782,20 @@
     </row>
     <row r="7" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L7" s="25">
-        <f>C3+D3+E3</f>
+        <f t="shared" si="4"/>
         <v>224</v>
       </c>
       <c r="M7" s="21">
-        <f>D3+E3+F3</f>
+        <f t="shared" si="4"/>
         <v>448</v>
       </c>
       <c r="N7" s="26">
-        <f>E3+F3+G3</f>
+        <f t="shared" si="4"/>
         <v>896</v>
       </c>
     </row>
     <row r="8" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="47" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="22">
@@ -1751,52 +1803,52 @@
         <v>4161</v>
       </c>
       <c r="D8" s="23">
-        <f t="shared" ref="D8:E10" si="4">D2+E3+F4</f>
+        <f t="shared" ref="D8:E10" si="5">D2+E3+F4</f>
         <v>8322</v>
       </c>
       <c r="E8" s="12">
+        <f t="shared" si="5"/>
+        <v>16644</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="22">
+        <f t="shared" ref="H8:J10" si="6">C4+D3+E2</f>
+        <v>1092</v>
+      </c>
+      <c r="I8" s="23">
+        <f t="shared" si="6"/>
+        <v>2184</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="6"/>
+        <v>4368</v>
+      </c>
+      <c r="L8" s="25">
         <f t="shared" si="4"/>
-        <v>16644</v>
-      </c>
-      <c r="G8" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="22">
-        <f>C4+D3+E2</f>
-        <v>1092</v>
-      </c>
-      <c r="I8" s="23">
-        <f>D4+E3+F2</f>
-        <v>2184</v>
-      </c>
-      <c r="J8" s="12">
-        <f>E4+F3+G2</f>
-        <v>4368</v>
-      </c>
-      <c r="L8" s="25">
-        <f>C4+D4+E4</f>
         <v>7168</v>
       </c>
       <c r="M8" s="21">
-        <f>D4+E4+F4</f>
+        <f t="shared" si="4"/>
         <v>14336</v>
       </c>
       <c r="N8" s="26">
-        <f>E4+F4+G4</f>
+        <f t="shared" si="4"/>
         <v>28672</v>
       </c>
-      <c r="Q8" s="56" t="str">
+      <c r="Q8" s="52" t="str">
         <f>CONCATENATE(C8, ",", D8, ",", E8, ",", C9, ",", D9, ",", E9, ",", C10, ",", D10, ",", E10)</f>
         <v>4161,8322,16644,133152,266304,532608,4260864,8521728,17043456</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="29">
-        <f t="shared" ref="C9:C10" si="5">C3+D4+E5</f>
+        <f t="shared" ref="C9:C10" si="7">C3+D4+E5</f>
         <v>133152</v>
       </c>
       <c r="D9" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>266304</v>
       </c>
       <c r="E9" s="26">
@@ -1804,69 +1856,69 @@
         <v>532608</v>
       </c>
       <c r="H9" s="25">
-        <f>C5+D4+E3</f>
+        <f t="shared" si="6"/>
         <v>34944</v>
       </c>
       <c r="I9" s="21">
-        <f>D5+E4+F3</f>
+        <f t="shared" si="6"/>
         <v>69888</v>
       </c>
       <c r="J9" s="26">
-        <f>E5+F4+G3</f>
+        <f t="shared" si="6"/>
         <v>139776</v>
       </c>
       <c r="L9" s="25">
-        <f>C5+D5+E5</f>
+        <f t="shared" si="4"/>
         <v>229376</v>
       </c>
       <c r="M9" s="21">
-        <f>D5+E5+F5</f>
+        <f t="shared" si="4"/>
         <v>458752</v>
       </c>
       <c r="N9" s="26">
-        <f>E5+F5+G5</f>
+        <f t="shared" si="4"/>
         <v>917504</v>
       </c>
-      <c r="Q9" s="56" t="str">
-        <f>CONCATENATE(H8, ",", I8, ",", J8, ",", H9, ",", I9, ",", J9, ",", I10, ",", J10)</f>
-        <v>1092,2184,4368,34944,69888,139776,2236416,4472832</v>
+      <c r="Q9" s="52" t="str">
+        <f>CONCATENATE(H8, ",", I8, ",", J8, ",", H9, ",", I9, ",", J9, ",", I10, ",", J10, ",", H10)</f>
+        <v>1092,2184,4368,34944,69888,139776,2236416,4472832,1118208</v>
       </c>
     </row>
     <row r="10" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="8">
+        <f t="shared" si="7"/>
+        <v>4260864</v>
+      </c>
+      <c r="D10" s="9">
         <f t="shared" si="5"/>
-        <v>4260864</v>
-      </c>
-      <c r="D10" s="9">
+        <v>8521728</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="5"/>
+        <v>17043456</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="6"/>
+        <v>1118208</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="6"/>
+        <v>2236416</v>
+      </c>
+      <c r="J10" s="30">
+        <f t="shared" si="6"/>
+        <v>4472832</v>
+      </c>
+      <c r="L10" s="8">
         <f t="shared" si="4"/>
-        <v>8521728</v>
-      </c>
-      <c r="E10" s="24">
+        <v>7340032</v>
+      </c>
+      <c r="M10" s="9">
         <f t="shared" si="4"/>
-        <v>17043456</v>
-      </c>
-      <c r="H10" s="8">
-        <f>C6+D5+E4</f>
-        <v>1118208</v>
-      </c>
-      <c r="I10" s="9">
-        <f>D6+E5+F4</f>
-        <v>2236416</v>
-      </c>
-      <c r="J10" s="30">
-        <f>E6+F5+G4</f>
-        <v>4472832</v>
-      </c>
-      <c r="L10" s="8">
-        <f>C6+D6+E6</f>
-        <v>7340032</v>
-      </c>
-      <c r="M10" s="9">
-        <f>D6+E6+F6</f>
         <v>14680064</v>
       </c>
       <c r="N10" s="24">
-        <f>E6+F6+G6</f>
+        <f t="shared" si="4"/>
         <v>29360128</v>
       </c>
     </row>
@@ -1876,47 +1928,47 @@
       </c>
       <c r="Q11" s="40" t="str">
         <f>CONCATENATE(Q2, ",", Q3, ",", Q4, ",", Q6, ",", R6, ",", S6, ",", Q8, ",", Q9)</f>
-        <v>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832</v>
+        <v>1057,2114,4228,8456,16912,33824,67648,135296,270592,541184,1082368,2164736,4329472,8658944,17317888,7,224,7168,229376,7340032,14,448,14336,458752,14680064,28,896,28672,917504,29360128,4161,8322,16644,133152,266304,532608,4260864,8521728,17043456,1092,2184,4368,34944,69888,139776,2236416,4472832,1118208</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="97" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P12" s="21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="41" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="55"/>
+      <c r="C14" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
     </row>
     <row r="15" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="11">
@@ -1927,23 +1979,23 @@
         <f>D2+E3+F4+G5</f>
         <v>532610</v>
       </c>
-      <c r="H15" s="45" t="s">
-        <v>16</v>
+      <c r="H15" s="44" t="s">
+        <v>14</v>
       </c>
       <c r="I15" s="11">
         <f>C2+C3+C4+C5</f>
         <v>33825</v>
       </c>
       <c r="J15" s="11">
-        <f t="shared" ref="J15:L15" si="6">D2+D3+D4+D5</f>
+        <f t="shared" ref="J15:L15" si="8">D2+D3+D4+D5</f>
         <v>67650</v>
       </c>
       <c r="K15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>135300</v>
       </c>
       <c r="L15" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>270600</v>
       </c>
       <c r="M15" s="11">
@@ -1972,15 +2024,15 @@
         <v>1082400</v>
       </c>
       <c r="J16" s="11">
-        <f t="shared" ref="J16" si="7">D3+D4+D5+D6</f>
+        <f t="shared" ref="J16" si="9">D3+D4+D5+D6</f>
         <v>2164800</v>
       </c>
       <c r="K16" s="11">
-        <f t="shared" ref="K16" si="8">E3+E4+E5+E6</f>
+        <f t="shared" ref="K16" si="10">E3+E4+E5+E6</f>
         <v>4329600</v>
       </c>
       <c r="L16" s="11">
-        <f t="shared" ref="L16" si="9">F3+F4+F5+F6</f>
+        <f t="shared" ref="L16" si="11">F3+F4+F5+F6</f>
         <v>8659200</v>
       </c>
       <c r="M16" s="11">
@@ -1996,7 +2048,7 @@
       </c>
     </row>
     <row r="17" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2">
@@ -2007,7 +2059,7 @@
         <f>D5+E4+F3+G2</f>
         <v>69904</v>
       </c>
-      <c r="H17" s="46" t="s">
+      <c r="H17" s="45" t="s">
         <v>1</v>
       </c>
       <c r="I17" s="11">
@@ -2033,80 +2085,80 @@
         <v>2236928</v>
       </c>
       <c r="I18" s="11">
-        <f t="shared" ref="I18:J18" si="10">C3+D3+E3+F3</f>
+        <f t="shared" ref="I18:J18" si="12">C3+D3+E3+F3</f>
         <v>480</v>
       </c>
-      <c r="J18" s="54">
-        <f t="shared" si="10"/>
+      <c r="J18" s="50">
+        <f t="shared" si="12"/>
         <v>960</v>
       </c>
     </row>
     <row r="19" spans="3:17" ht="73" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I19" s="11">
-        <f t="shared" ref="I19:J19" si="11">C4+D4+E4+F4</f>
+        <f t="shared" ref="I19:J19" si="13">C4+D4+E4+F4</f>
         <v>15360</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>30720</v>
       </c>
       <c r="P19" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Q19" s="57" t="str">
+      <c r="Q19" s="53" t="str">
         <f>CONCATENATE(Q15,",",Q16,",",Q17)</f>
         <v>266305,532610,8521760,17043520,34952,69904,1118464,2236928,33825,67650,135300,270600,541200,1082400,2164800,4329600,8659200,17318400,15,30,480,960,15360,30720,491520,983040,15728640,31457280</v>
       </c>
     </row>
     <row r="20" spans="3:17" ht="73" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I20" s="11">
-        <f t="shared" ref="I20:J20" si="12">C5+D5+E5+F5</f>
+        <f t="shared" ref="I20:J20" si="14">C5+D5+E5+F5</f>
         <v>491520</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>983040</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q20" s="41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I21" s="11">
-        <f t="shared" ref="I21:J21" si="13">C6+D6+E6+F6</f>
+        <f t="shared" ref="I21:J21" si="15">C6+D6+E6+F6</f>
         <v>15728640</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>31457280</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="50"/>
+      <c r="C23" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="57"/>
     </row>
     <row r="24" spans="3:17" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="44" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="24">
@@ -2116,13 +2168,13 @@
       <c r="P24" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Q24" s="57" t="str">
+      <c r="Q24" s="53" t="str">
         <f>CONCATENATE(D24,",",D25,",",D26,",",E26,",",F26,",",G26,",",H26,",",D27,",",D28,",",D29,",",D30,",",D31)</f>
         <v>17043521,1118480,1082401,2164802,4329604,8659208,17318416,31,992,31744,1015808,32505856</v>
       </c>
     </row>
     <row r="25" spans="3:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="7">
@@ -2131,14 +2183,14 @@
       </c>
       <c r="K25" s="3"/>
       <c r="P25" s="21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q25" s="41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="44" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2">
@@ -2146,24 +2198,24 @@
         <v>1082401</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" ref="E26:H26" si="14">D2+D3+D4+D5+D6</f>
+        <f t="shared" ref="E26:H26" si="16">D2+D3+D4+D5+D6</f>
         <v>2164802</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4329604</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8659208</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>17318416</v>
       </c>
     </row>
     <row r="27" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="45" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="2">
@@ -2173,25 +2225,25 @@
     </row>
     <row r="28" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="2">
-        <f t="shared" ref="D28:D31" si="15">C3+D3+E3+F3+G3</f>
+        <f t="shared" ref="D28:D31" si="17">C3+D3+E3+F3+G3</f>
         <v>992</v>
       </c>
     </row>
     <row r="29" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>31744</v>
       </c>
     </row>
     <row r="30" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1015808</v>
       </c>
     </row>
     <row r="31" spans="3:17" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>32505856</v>
       </c>
     </row>
@@ -2204,6 +2256,8 @@
     <mergeCell ref="C14:M14"/>
     <mergeCell ref="N14:R14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="8" scale="39" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>